<commit_message>
RACI inseriti totali e corretto secondo indicazioni prof
</commit_message>
<xml_diff>
--- a/Fase_2/RACI.xlsx
+++ b/Fase_2/RACI.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\GestioneProgetti\Fase_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utente/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B72A60-ACF8-45CF-B2BF-8D63E15DC754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A243DFD-8B21-744B-AC73-927A4AB6CA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
+    <workbookView xWindow="15220" yWindow="500" windowWidth="13380" windowHeight="15720" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="68">
   <si>
     <t>1.1 Definizione degli obiettivi del progetto</t>
   </si>
@@ -226,15 +237,46 @@
   </si>
   <si>
     <t>A/C</t>
+  </si>
+  <si>
+    <t>Totale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -249,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -272,17 +314,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,23 +708,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9914445C-CD02-4581-B140-F9EDBB427865}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60:E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>56</v>
@@ -633,53 +742,49 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -687,7 +792,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -703,7 +808,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -719,7 +824,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -735,12 +840,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>62</v>
@@ -751,7 +856,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -760,16 +865,16 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -778,16 +883,14 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -795,24 +898,24 @@
         <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
@@ -823,7 +926,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -835,13 +938,13 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -857,7 +960,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -865,7 +968,7 @@
         <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
@@ -875,7 +978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -883,7 +986,7 @@
         <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>64</v>
@@ -895,7 +998,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -906,70 +1009,66 @@
         <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="9" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C20" s="10"/>
       <c r="D20" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -983,21 +1082,21 @@
         <v>64</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E22" s="3"/>
@@ -1005,23 +1104,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="D23" s="10"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1033,13 +1130,13 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1047,35 +1144,33 @@
         <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E26" s="7"/>
       <c r="F26" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1178,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>62</v>
@@ -1093,49 +1188,45 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B30" s="6"/>
       <c r="C30" s="3" t="s">
         <v>64</v>
       </c>
@@ -1145,7 +1236,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1156,14 +1247,14 @@
         <v>62</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1179,7 +1270,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -1197,7 +1288,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1206,14 +1297,14 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1224,14 +1315,14 @@
       <c r="D35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="11" t="s">
         <v>62</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1242,14 +1333,12 @@
       <c r="D36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E36" s="11"/>
       <c r="F36" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1258,14 +1347,12 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E37" s="11"/>
       <c r="F37" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1281,45 +1368,43 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="9" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B40" s="10"/>
       <c r="C40" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1330,65 +1415,63 @@
         <v>62</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>64</v>
@@ -1397,63 +1480,59 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C45" s="6"/>
       <c r="D45" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="D47" s="10"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -1469,7 +1548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -1480,14 +1559,14 @@
       <c r="D49" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -1498,14 +1577,12 @@
       <c r="D50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="E50" s="8"/>
       <c r="F50" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -1523,43 +1600,41 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="D53" s="13"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -1567,33 +1642,33 @@
         <v>66</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E55" s="7"/>
       <c r="F55" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -1605,13 +1680,13 @@
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -1619,19 +1694,62 @@
         <v>65</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" s="2">
+        <f>COUNTIF(B2:B57,"R/A")</f>
+        <v>10</v>
+      </c>
+      <c r="C58" s="2">
+        <f>COUNTIF(C2:C57,"r")</f>
+        <v>11</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" ref="D58:E58" si="0">COUNTIF(D2:D57,"r")</f>
+        <v>9</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="2">
+        <f>SUM(B58:E58)</f>
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E25:E26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>